<commit_message>
Refactor CPUInfoExcel to update initial values for cryptographic keys; enhance memory handling in PresentacionView; adjust window position in config.json; update binary files for cpu_info_excel and table_data.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,40 +413,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BN64"/>
+  <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="18.7109375" customWidth="1" min="1" max="1"/>
-    <col width="29.140625" customWidth="1" min="2" max="2"/>
-    <col width="27.7109375" customWidth="1" min="4" max="4"/>
-    <col width="28.85546875" customWidth="1" min="5" max="5"/>
-    <col width="23.28515625" customWidth="1" min="7" max="7"/>
-    <col width="22.42578125" customWidth="1" min="8" max="8"/>
-    <col width="27.42578125" customWidth="1" min="10" max="10"/>
-    <col width="23.42578125" customWidth="1" min="11" max="11"/>
-    <col width="24.140625" customWidth="1" min="13" max="13"/>
-    <col width="22.28515625" customWidth="1" min="14" max="14"/>
-    <col width="27" customWidth="1" min="15" max="15"/>
-    <col width="22.42578125" customWidth="1" min="16" max="16"/>
-    <col width="19.140625" customWidth="1" min="17" max="17"/>
-    <col width="19.42578125" customWidth="1" min="18" max="18"/>
-    <col width="16.85546875" customWidth="1" min="19" max="19"/>
-    <col width="16.7109375" customWidth="1" min="20" max="20"/>
-    <col width="14.42578125" customWidth="1" min="22" max="22"/>
-    <col width="21" customWidth="1" min="23" max="23"/>
-    <col width="11" customWidth="1" min="24" max="24"/>
-    <col width="17.7109375" customWidth="1" min="25" max="25"/>
-    <col width="21.42578125" customWidth="1" min="26" max="26"/>
-    <col width="18.28515625" customWidth="1" min="28" max="28"/>
-    <col width="20" customWidth="1" min="29" max="29"/>
-    <col width="19" customWidth="1" min="31" max="31"/>
-    <col width="21.140625" customWidth="1" min="32" max="32"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -523,31 +497,11 @@
           <t>String: 'P1'</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000001</t>
-        </is>
-      </c>
       <c r="Y1" t="inlineStr">
         <is>
           <t>String: 'k0.0'</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>String: 'G0'</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
       <c r="AE1" t="inlineStr">
         <is>
           <t>String: 'D_Mem0'</t>
@@ -555,7 +509,7 @@
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x486F6C61</t>
         </is>
       </c>
     </row>
@@ -635,29 +589,19 @@
           <t>String: 'P2'</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000010</t>
-        </is>
-      </c>
       <c r="Y2" t="inlineStr">
         <is>
           <t>String: 'k0.1'</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>String: 'G1'</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>String: 'D_Mem1'</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Hex: 0x20736F79</t>
         </is>
       </c>
     </row>
@@ -737,29 +681,19 @@
           <t>String: 'P3'</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000011</t>
-        </is>
-      </c>
       <c r="Y3" t="inlineStr">
         <is>
           <t>String: 'k0.2'</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>String: 'G2'</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>String: 'D_Mem2'</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Hex: 0x20756E20</t>
         </is>
       </c>
     </row>
@@ -839,29 +773,19 @@
           <t>String: 'P4'</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000100</t>
-        </is>
-      </c>
       <c r="Y4" t="inlineStr">
         <is>
           <t>String: 'k0.3'</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>String: 'G3'</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>String: 'D_Mem3'</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Hex: 0x656A656D</t>
         </is>
       </c>
     </row>
@@ -931,29 +855,19 @@
           <t>String: 'P5'</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000101</t>
-        </is>
-      </c>
       <c r="Y5" t="inlineStr">
         <is>
           <t>String: 'k1.0'</t>
         </is>
       </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>String: 'G4'</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>String: 'D_Mem4'</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Hex: 0x706C6F00</t>
         </is>
       </c>
     </row>
@@ -1023,27 +937,17 @@
           <t>String: 'P6'</t>
         </is>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000110</t>
-        </is>
-      </c>
       <c r="Y6" t="inlineStr">
         <is>
           <t>String: 'k1.1'</t>
         </is>
       </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>String: 'G5'</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>String: 'D_Mem5'</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
         <is>
           <t>Hex: 0x00000000</t>
         </is>
@@ -1115,29 +1019,9 @@
           <t>String: 'P7'</t>
         </is>
       </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000111</t>
-        </is>
-      </c>
       <c r="Y7" t="inlineStr">
         <is>
           <t>String: 'k1.2'</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>String: 'G6'</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -1207,29 +1091,9 @@
           <t>String: 'P8'</t>
         </is>
       </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>Hex: 0x00001000</t>
-        </is>
-      </c>
       <c r="Y8" t="inlineStr">
         <is>
           <t>String: 'k1.3'</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>String: 'G7'</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -1299,21 +1163,6 @@
           <t>String: 'k2.0'</t>
         </is>
       </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>String: 'G8'</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="D10" t="inlineStr">
@@ -1381,21 +1230,6 @@
           <t>String: 'k2.1'</t>
         </is>
       </c>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>String: 'G9'</t>
-        </is>
-      </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="D11" t="inlineStr">
@@ -1453,21 +1287,6 @@
           <t>String: 'k2.2'</t>
         </is>
       </c>
-      <c r="Z11" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>String: 'G10'</t>
-        </is>
-      </c>
-      <c r="AC11" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="D12" t="inlineStr">
@@ -1525,21 +1344,6 @@
           <t>String: 'k2.3'</t>
         </is>
       </c>
-      <c r="Z12" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB12" t="inlineStr">
-        <is>
-          <t>String: 'G11'</t>
-        </is>
-      </c>
-      <c r="AC12" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="D13" t="inlineStr">
@@ -1587,21 +1391,6 @@
           <t>String: 'k3.0'</t>
         </is>
       </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>String: 'G12'</t>
-        </is>
-      </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="D14" t="inlineStr">
@@ -1649,21 +1438,6 @@
           <t>String: 'k3.1'</t>
         </is>
       </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB14" t="inlineStr">
-        <is>
-          <t>String: 'G13'</t>
-        </is>
-      </c>
-      <c r="AC14" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="D15" t="inlineStr">
@@ -1711,21 +1485,6 @@
           <t>String: 'k3.2'</t>
         </is>
       </c>
-      <c r="Z15" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>String: 'G14'</t>
-        </is>
-      </c>
-      <c r="AC15" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="D16" t="inlineStr">
@@ -1773,21 +1532,6 @@
           <t>String: 'k3.3'</t>
         </is>
       </c>
-      <c r="Z16" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="AB16" t="inlineStr">
-        <is>
-          <t>String: 'G15'</t>
-        </is>
-      </c>
-      <c r="AC16" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="D17" t="inlineStr">
@@ -1820,16 +1564,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t>String: 'G16'</t>
-        </is>
-      </c>
-      <c r="AC17" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
@@ -1862,16 +1596,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB18" t="inlineStr">
-        <is>
-          <t>String: 'G17'</t>
-        </is>
-      </c>
-      <c r="AC18" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="D19" t="inlineStr">
@@ -1894,16 +1618,6 @@
           <t>Binary: 0b0000</t>
         </is>
       </c>
-      <c r="AB19" t="inlineStr">
-        <is>
-          <t>String: 'G18'</t>
-        </is>
-      </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
@@ -1926,21 +1640,6 @@
           <t>Binary: 0b0000</t>
         </is>
       </c>
-      <c r="AB20" t="inlineStr">
-        <is>
-          <t>String: 'G19'</t>
-        </is>
-      </c>
-      <c r="AC20" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-      <c r="BN20" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="D21" t="inlineStr">
@@ -1963,16 +1662,6 @@
           <t>Binary: 0b0</t>
         </is>
       </c>
-      <c r="AB21" t="inlineStr">
-        <is>
-          <t>String: 'G20'</t>
-        </is>
-      </c>
-      <c r="AC21" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="D22" t="inlineStr">
@@ -1995,16 +1684,6 @@
           <t>Binary: 0b0</t>
         </is>
       </c>
-      <c r="AB22" t="inlineStr">
-        <is>
-          <t>String: 'G21'</t>
-        </is>
-      </c>
-      <c r="AC22" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
@@ -2027,16 +1706,6 @@
           <t>Binary: 0b00</t>
         </is>
       </c>
-      <c r="AB23" t="inlineStr">
-        <is>
-          <t>String: 'G22'</t>
-        </is>
-      </c>
-      <c r="AC23" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="D24" t="inlineStr">
@@ -2059,16 +1728,6 @@
           <t>Binary: 0b0000</t>
         </is>
       </c>
-      <c r="AB24" t="inlineStr">
-        <is>
-          <t>String: 'G23'</t>
-        </is>
-      </c>
-      <c r="AC24" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="D25" t="inlineStr">
@@ -2091,16 +1750,6 @@
           <t>Binary: 0b0000</t>
         </is>
       </c>
-      <c r="AB25" t="inlineStr">
-        <is>
-          <t>String: 'G24'</t>
-        </is>
-      </c>
-      <c r="AC25" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="D26" t="inlineStr">
@@ -2123,16 +1772,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB26" t="inlineStr">
-        <is>
-          <t>String: 'G25'</t>
-        </is>
-      </c>
-      <c r="AC26" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="D27" t="inlineStr">
@@ -2155,16 +1794,6 @@
           <t>Binary: 0b0</t>
         </is>
       </c>
-      <c r="AB27" t="inlineStr">
-        <is>
-          <t>String: 'G26'</t>
-        </is>
-      </c>
-      <c r="AC27" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
@@ -2177,16 +1806,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB28" t="inlineStr">
-        <is>
-          <t>String: 'G27'</t>
-        </is>
-      </c>
-      <c r="AC28" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
@@ -2199,16 +1818,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB29" t="inlineStr">
-        <is>
-          <t>String: 'G28'</t>
-        </is>
-      </c>
-      <c r="AC29" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
@@ -2221,16 +1830,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB30" t="inlineStr">
-        <is>
-          <t>String: 'G29'</t>
-        </is>
-      </c>
-      <c r="AC30" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
@@ -2243,16 +1842,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB31" t="inlineStr">
-        <is>
-          <t>String: 'G30'</t>
-        </is>
-      </c>
-      <c r="AC31" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
@@ -2265,16 +1854,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB32" t="inlineStr">
-        <is>
-          <t>String: 'G31'</t>
-        </is>
-      </c>
-      <c r="AC32" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
@@ -2287,16 +1866,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB33" t="inlineStr">
-        <is>
-          <t>String: 'G32'</t>
-        </is>
-      </c>
-      <c r="AC33" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
@@ -2309,16 +1878,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB34" t="inlineStr">
-        <is>
-          <t>String: 'G33'</t>
-        </is>
-      </c>
-      <c r="AC34" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
@@ -2331,16 +1890,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB35" t="inlineStr">
-        <is>
-          <t>String: 'G34'</t>
-        </is>
-      </c>
-      <c r="AC35" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
@@ -2353,16 +1902,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB36" t="inlineStr">
-        <is>
-          <t>String: 'G35'</t>
-        </is>
-      </c>
-      <c r="AC36" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
@@ -2375,52 +1914,6 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
-      <c r="AB37" t="inlineStr">
-        <is>
-          <t>String: 'G36'</t>
-        </is>
-      </c>
-      <c r="AC37" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="AB38" t="inlineStr">
-        <is>
-          <t>String: 'G37'</t>
-        </is>
-      </c>
-      <c r="AC38" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="AB39" t="inlineStr">
-        <is>
-          <t>String: 'G38'</t>
-        </is>
-      </c>
-      <c r="AC39" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="AB40" t="inlineStr">
-        <is>
-          <t>String: 'G39'</t>
-        </is>
-      </c>
-      <c r="AC40" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2448,16 +1941,6 @@
           <t>String: 'WriteBack:'</t>
         </is>
       </c>
-      <c r="AB41" t="inlineStr">
-        <is>
-          <t>String: 'G40'</t>
-        </is>
-      </c>
-      <c r="AC41" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2490,29 +1973,9 @@
           <t>String: 'Timer Value'</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>Int: 0d0</t>
-        </is>
-      </c>
       <c r="R42" t="inlineStr">
         <is>
           <t>String: 'Intentos'</t>
-        </is>
-      </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>Binary: 0b0000</t>
-        </is>
-      </c>
-      <c r="AB42" t="inlineStr">
-        <is>
-          <t>String: 'G41'</t>
-        </is>
-      </c>
-      <c r="AC42" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -2522,281 +1985,11 @@
           <t>String: 'Block Status In'</t>
         </is>
       </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>Binary: 0b00000000</t>
-        </is>
-      </c>
-      <c r="AB43" t="inlineStr">
-        <is>
-          <t>String: 'G42'</t>
-        </is>
-      </c>
-      <c r="AC43" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="O44" t="inlineStr">
         <is>
           <t>String: 'Block Status Out'</t>
-        </is>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>Binary: 0b00000000</t>
-        </is>
-      </c>
-      <c r="AB44" t="inlineStr">
-        <is>
-          <t>String: 'G43'</t>
-        </is>
-      </c>
-      <c r="AC44" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="AB45" t="inlineStr">
-        <is>
-          <t>String: 'G44'</t>
-        </is>
-      </c>
-      <c r="AC45" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="AB46" t="inlineStr">
-        <is>
-          <t>String: 'G45'</t>
-        </is>
-      </c>
-      <c r="AC46" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="AB47" t="inlineStr">
-        <is>
-          <t>String: 'G46'</t>
-        </is>
-      </c>
-      <c r="AC47" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="AB48" t="inlineStr">
-        <is>
-          <t>String: 'G47'</t>
-        </is>
-      </c>
-      <c r="AC48" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="AB49" t="inlineStr">
-        <is>
-          <t>String: 'G48'</t>
-        </is>
-      </c>
-      <c r="AC49" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="AB50" t="inlineStr">
-        <is>
-          <t>String: 'G49'</t>
-        </is>
-      </c>
-      <c r="AC50" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="AB51" t="inlineStr">
-        <is>
-          <t>String: 'G50'</t>
-        </is>
-      </c>
-      <c r="AC51" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="AB52" t="inlineStr">
-        <is>
-          <t>String: 'G51'</t>
-        </is>
-      </c>
-      <c r="AC52" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="AB53" t="inlineStr">
-        <is>
-          <t>String: 'G52'</t>
-        </is>
-      </c>
-      <c r="AC53" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="AB54" t="inlineStr">
-        <is>
-          <t>String: 'G53'</t>
-        </is>
-      </c>
-      <c r="AC54" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="AB55" t="inlineStr">
-        <is>
-          <t>String: 'G54'</t>
-        </is>
-      </c>
-      <c r="AC55" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="AB56" t="inlineStr">
-        <is>
-          <t>String: 'G55'</t>
-        </is>
-      </c>
-      <c r="AC56" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="AB57" t="inlineStr">
-        <is>
-          <t>String: 'G56'</t>
-        </is>
-      </c>
-      <c r="AC57" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="AB58" t="inlineStr">
-        <is>
-          <t>String: 'G57'</t>
-        </is>
-      </c>
-      <c r="AC58" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="AB59" t="inlineStr">
-        <is>
-          <t>String: 'G58'</t>
-        </is>
-      </c>
-      <c r="AC59" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="AB60" t="inlineStr">
-        <is>
-          <t>String: 'G59'</t>
-        </is>
-      </c>
-      <c r="AC60" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="AB61" t="inlineStr">
-        <is>
-          <t>String: 'G60'</t>
-        </is>
-      </c>
-      <c r="AC61" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="AB62" t="inlineStr">
-        <is>
-          <t>String: 'G61'</t>
-        </is>
-      </c>
-      <c r="AC62" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="AB63" t="inlineStr">
-        <is>
-          <t>String: 'G62'</t>
-        </is>
-      </c>
-      <c r="AC63" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="AB64" t="inlineStr">
-        <is>
-          <t>String: 'G63'</t>
-        </is>
-      </c>
-      <c r="AC64" t="inlineStr">
-        <is>
-          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add dynamic memory binary and update main application structure
- Added new binary file `dynamic_mem.bin` containing a text excerpt from "Evangelio según Marcos" by Jorge Luis Borges.
- Introduced an encrypted version of the binary file as `dynamic_mem.enc`.
- Minor formatting adjustment in `main.py` to ensure consistent code style.
- Updated `table_data.xlsx` with new data.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -2,27 +2,34 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -46,11 +53,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +421,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF44"/>
+  <dimension ref="A1:IP68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="11.85546875" customWidth="1" min="27" max="27"/>
+    <col width="15" customWidth="1" min="28" max="28"/>
+    <col width="24.7109375" customWidth="1" min="29" max="29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -497,19 +510,29 @@
           <t>String: 'P1'</t>
         </is>
       </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000001</t>
+        </is>
+      </c>
       <c r="Y1" t="inlineStr">
         <is>
           <t>String: 'k0.0'</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>String: 'D_Mem0'</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>Hex: 0x486F6C61</t>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>String: 'G0'</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>Hex: 0x062EFFFF</t>
         </is>
       </c>
     </row>
@@ -589,19 +612,29 @@
           <t>String: 'P2'</t>
         </is>
       </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000010</t>
+        </is>
+      </c>
       <c r="Y2" t="inlineStr">
         <is>
           <t>String: 'k0.1'</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>String: 'D_Mem1'</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>Hex: 0x20736F79</t>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>String: 'G1'</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -681,19 +714,29 @@
           <t>String: 'P3'</t>
         </is>
       </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000011</t>
+        </is>
+      </c>
       <c r="Y3" t="inlineStr">
         <is>
           <t>String: 'k0.2'</t>
         </is>
       </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>String: 'D_Mem2'</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>Hex: 0x20756E20</t>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>String: 'G2'</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -773,19 +816,29 @@
           <t>String: 'P4'</t>
         </is>
       </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000100</t>
+        </is>
+      </c>
       <c r="Y4" t="inlineStr">
         <is>
           <t>String: 'k0.3'</t>
         </is>
       </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>String: 'D_Mem3'</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>Hex: 0x656A656D</t>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>String: 'G3'</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -855,19 +908,29 @@
           <t>String: 'P5'</t>
         </is>
       </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000101</t>
+        </is>
+      </c>
       <c r="Y5" t="inlineStr">
         <is>
           <t>String: 'k1.0'</t>
         </is>
       </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>String: 'D_Mem4'</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>Hex: 0x706C6F00</t>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>String: 'G4'</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -937,17 +1000,27 @@
           <t>String: 'P6'</t>
         </is>
       </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000110</t>
+        </is>
+      </c>
       <c r="Y6" t="inlineStr">
         <is>
           <t>String: 'k1.1'</t>
         </is>
       </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>String: 'D_Mem5'</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>String: 'G5'</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
         <is>
           <t>Hex: 0x00000000</t>
         </is>
@@ -1019,11 +1092,32 @@
           <t>String: 'P7'</t>
         </is>
       </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000111</t>
+        </is>
+      </c>
       <c r="Y7" t="inlineStr">
         <is>
           <t>String: 'k1.2'</t>
         </is>
       </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>String: 'G6'</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AD7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="D8" t="inlineStr">
@@ -1091,9 +1185,29 @@
           <t>String: 'P8'</t>
         </is>
       </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Hex: 0x00001000</t>
+        </is>
+      </c>
       <c r="Y8" t="inlineStr">
         <is>
           <t>String: 'k1.3'</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>String: 'G7'</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -1163,6 +1277,21 @@
           <t>String: 'k2.0'</t>
         </is>
       </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>String: 'G8'</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="D10" t="inlineStr">
@@ -1230,6 +1359,21 @@
           <t>String: 'k2.1'</t>
         </is>
       </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>String: 'G9'</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="D11" t="inlineStr">
@@ -1287,6 +1431,21 @@
           <t>String: 'k2.2'</t>
         </is>
       </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>String: 'G10'</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="D12" t="inlineStr">
@@ -1344,6 +1503,21 @@
           <t>String: 'k2.3'</t>
         </is>
       </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>String: 'G11'</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="D13" t="inlineStr">
@@ -1391,6 +1565,21 @@
           <t>String: 'k3.0'</t>
         </is>
       </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>String: 'G12'</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="D14" t="inlineStr">
@@ -1438,6 +1627,21 @@
           <t>String: 'k3.1'</t>
         </is>
       </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>String: 'G13'</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="D15" t="inlineStr">
@@ -1485,6 +1689,21 @@
           <t>String: 'k3.2'</t>
         </is>
       </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>String: 'G14'</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="D16" t="inlineStr">
@@ -1532,6 +1751,21 @@
           <t>String: 'k3.3'</t>
         </is>
       </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>String: 'G15'</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="D17" t="inlineStr">
@@ -1564,6 +1798,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>String: 'G16'</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
@@ -1596,6 +1840,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>String: 'G17'</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="D19" t="inlineStr">
@@ -1618,6 +1872,16 @@
           <t>Binary: 0b0000</t>
         </is>
       </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>String: 'G18'</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
@@ -1640,6 +1904,16 @@
           <t>Binary: 0b0000</t>
         </is>
       </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>String: 'G19'</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="D21" t="inlineStr">
@@ -1662,6 +1936,16 @@
           <t>Binary: 0b0</t>
         </is>
       </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>String: 'G20'</t>
+        </is>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="D22" t="inlineStr">
@@ -1684,6 +1968,16 @@
           <t>Binary: 0b0</t>
         </is>
       </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>String: 'G21'</t>
+        </is>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
@@ -1706,6 +2000,16 @@
           <t>Binary: 0b00</t>
         </is>
       </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>String: 'G22'</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="D24" t="inlineStr">
@@ -1728,6 +2032,16 @@
           <t>Binary: 0b0000</t>
         </is>
       </c>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>String: 'G23'</t>
+        </is>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="D25" t="inlineStr">
@@ -1750,6 +2064,16 @@
           <t>Binary: 0b0000</t>
         </is>
       </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>String: 'G24'</t>
+        </is>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="D26" t="inlineStr">
@@ -1772,6 +2096,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>String: 'G25'</t>
+        </is>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="D27" t="inlineStr">
@@ -1794,6 +2128,16 @@
           <t>Binary: 0b0</t>
         </is>
       </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>String: 'G26'</t>
+        </is>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
@@ -1806,6 +2150,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>String: 'G27'</t>
+        </is>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
@@ -1818,6 +2172,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>String: 'G28'</t>
+        </is>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
@@ -1830,6 +2194,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>String: 'G29'</t>
+        </is>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="D31" t="inlineStr">
@@ -1842,6 +2216,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>String: 'G30'</t>
+        </is>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
@@ -1854,6 +2238,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>String: 'G31'</t>
+        </is>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="D33" t="inlineStr">
@@ -1866,6 +2260,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t>String: 'G32'</t>
+        </is>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="D34" t="inlineStr">
@@ -1878,6 +2282,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>String: 'G33'</t>
+        </is>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
@@ -1890,6 +2304,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>String: 'G34'</t>
+        </is>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="D36" t="inlineStr">
@@ -1902,6 +2326,16 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB36" t="inlineStr">
+        <is>
+          <t>String: 'G35'</t>
+        </is>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="D37" t="inlineStr">
@@ -1914,6 +2348,52 @@
           <t>Hex: 0x00000000</t>
         </is>
       </c>
+      <c r="AB37" t="inlineStr">
+        <is>
+          <t>String: 'G36'</t>
+        </is>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="AB38" t="inlineStr">
+        <is>
+          <t>String: 'G37'</t>
+        </is>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="AB39" t="inlineStr">
+        <is>
+          <t>String: 'G38'</t>
+        </is>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="AB40" t="inlineStr">
+        <is>
+          <t>String: 'G39'</t>
+        </is>
+      </c>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1941,6 +2421,16 @@
           <t>String: 'WriteBack:'</t>
         </is>
       </c>
+      <c r="AB41" t="inlineStr">
+        <is>
+          <t>String: 'G40'</t>
+        </is>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1973,9 +2463,29 @@
           <t>String: 'Timer Value'</t>
         </is>
       </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Int: 0d0</t>
+        </is>
+      </c>
       <c r="R42" t="inlineStr">
         <is>
           <t>String: 'Intentos'</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>Binary: 0b0000</t>
+        </is>
+      </c>
+      <c r="AB42" t="inlineStr">
+        <is>
+          <t>String: 'G41'</t>
+        </is>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -1985,11 +2495,288 @@
           <t>String: 'Block Status In'</t>
         </is>
       </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Binary: 0b00000000</t>
+        </is>
+      </c>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>String: 'G42'</t>
+        </is>
+      </c>
+      <c r="AC43" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="O44" t="inlineStr">
         <is>
           <t>String: 'Block Status Out'</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Binary: 0b00000000</t>
+        </is>
+      </c>
+      <c r="AB44" t="inlineStr">
+        <is>
+          <t>String: 'G43'</t>
+        </is>
+      </c>
+      <c r="AC44" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="AB45" t="inlineStr">
+        <is>
+          <t>String: 'G44'</t>
+        </is>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="AB46" t="inlineStr">
+        <is>
+          <t>String: 'G45'</t>
+        </is>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="AB47" t="inlineStr">
+        <is>
+          <t>String: 'G46'</t>
+        </is>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="AB48" t="inlineStr">
+        <is>
+          <t>String: 'G47'</t>
+        </is>
+      </c>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="AB49" t="inlineStr">
+        <is>
+          <t>String: 'G48'</t>
+        </is>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="AB50" t="inlineStr">
+        <is>
+          <t>String: 'G49'</t>
+        </is>
+      </c>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="AB51" t="inlineStr">
+        <is>
+          <t>String: 'G50'</t>
+        </is>
+      </c>
+      <c r="AC51" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="AB52" t="inlineStr">
+        <is>
+          <t>String: 'G51'</t>
+        </is>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="AB53" t="inlineStr">
+        <is>
+          <t>String: 'G52'</t>
+        </is>
+      </c>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="AB54" t="inlineStr">
+        <is>
+          <t>String: 'G53'</t>
+        </is>
+      </c>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="AB55" t="inlineStr">
+        <is>
+          <t>String: 'G54'</t>
+        </is>
+      </c>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="AB56" t="inlineStr">
+        <is>
+          <t>String: 'G55'</t>
+        </is>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="AB57" t="inlineStr">
+        <is>
+          <t>String: 'G56'</t>
+        </is>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="AB58" t="inlineStr">
+        <is>
+          <t>String: 'G57'</t>
+        </is>
+      </c>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="AB59" t="inlineStr">
+        <is>
+          <t>String: 'G58'</t>
+        </is>
+      </c>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="AB60" t="inlineStr">
+        <is>
+          <t>String: 'G59'</t>
+        </is>
+      </c>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="AB61" t="inlineStr">
+        <is>
+          <t>String: 'G60'</t>
+        </is>
+      </c>
+      <c r="AC61" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="AB62" t="inlineStr">
+        <is>
+          <t>String: 'G61'</t>
+        </is>
+      </c>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="AB63" t="inlineStr">
+        <is>
+          <t>String: 'G62'</t>
+        </is>
+      </c>
+      <c r="AC63" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="AB64" t="inlineStr">
+        <is>
+          <t>String: 'G63'</t>
+        </is>
+      </c>
+      <c r="AC64" t="inlineStr">
+        <is>
+          <t>Hex: 0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="IP68" t="inlineStr">
+        <is>
+          <t>a</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add instruction memory reading functionality and reset memory button in CompiladorView; update window position in config.json
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -427,7 +427,7 @@
       <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.140625" customWidth="1" min="25" max="25"/>
     <col width="23" customWidth="1" min="26" max="26"/>
@@ -524,7 +524,7 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>Hex: 0xADBEEF00</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>Int: 0d-502415</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
@@ -830,7 +830,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
@@ -922,7 +922,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
@@ -1014,7 +1014,7 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB8" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB12" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB13" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB14" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB15" t="inlineStr">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB16" t="inlineStr">

</xml_diff>

<commit_message>
Add interactive CPU pipeline diagram component with zoom and pan functionality
- Implemented InteractiveDiagram class for creating a scalable and draggable canvas.
- Developed CPUPipelineDiagram class to visualize CPU pipeline stages including Fetch, Decode, Execute, Memory, and WriteBack.
- Added methods for drawing various components such as multiplexers, flip-flops, ALU, and instruction boxes.
- Integrated signal management to update and display CPU signals dynamically.
- Enhanced theme support for better visual consistency.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -423,12 +423,30 @@
   </sheetPr>
   <dimension ref="A1:IP68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
+    <col width="18.42578125" customWidth="1" min="1" max="1"/>
+    <col width="26.140625" customWidth="1" min="2" max="2"/>
+    <col width="28.140625" customWidth="1" min="4" max="4"/>
+    <col width="24.28515625" customWidth="1" min="5" max="5"/>
+    <col width="25.140625" customWidth="1" min="7" max="7"/>
+    <col width="19.85546875" customWidth="1" min="8" max="8"/>
+    <col width="24.28515625" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="25.140625" customWidth="1" min="13" max="13"/>
+    <col width="18.85546875" customWidth="1" min="14" max="14"/>
+    <col width="28.140625" customWidth="1" min="15" max="15"/>
+    <col width="20.7109375" customWidth="1" min="16" max="16"/>
+    <col width="19.28515625" customWidth="1" min="17" max="17"/>
+    <col width="19.140625" customWidth="1" min="18" max="18"/>
+    <col width="18.85546875" customWidth="1" min="19" max="19"/>
+    <col width="16.42578125" customWidth="1" min="20" max="20"/>
+    <col width="11.5703125" customWidth="1" min="22" max="22"/>
+    <col width="17.140625" customWidth="1" min="23" max="23"/>
     <col width="15.140625" customWidth="1" min="25" max="25"/>
     <col width="23" customWidth="1" min="26" max="26"/>
     <col width="11.85546875" customWidth="1" min="27" max="27"/>
@@ -454,7 +472,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Hex: 0x300000000000000</t>
+          <t>Hex: 0x3000000000000000</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -524,7 +542,7 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
@@ -626,7 +644,7 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
@@ -728,7 +746,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
@@ -750,7 +768,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hex: 0x300000000000000</t>
+          <t>Hex: 0x3000000000000000</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -830,7 +848,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">

</xml_diff>

<commit_message>
Refactor instruction handling in CPUView; update window position in config.json for improved layout
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -2463,22 +2463,22 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>String: 'ADD R1, R2, R1'</t>
+          <t>String: 'NOP'</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>String: 'ADD R1, R2, R1'</t>
+          <t>String: 'NOP'</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>String: 'ADD R1, R2, R1'</t>
+          <t>String: 'NOP'</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>String: 'ADD R1, R2, R1'</t>
+          <t>String: 'NOP'</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">

</xml_diff>

<commit_message>
Integration of some elements
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -624,7 +624,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000598</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
@@ -2458,17 +2458,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>String: 'MOVI R1, #150'</t>
+          <t>String: 'NOP'</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>String: 'MOVI R1, #150'</t>
+          <t>String: 'NOP'</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>String: 'MOVI R1, #150'</t>
+          <t>String: 'NOP'</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">

</xml_diff>

<commit_message>
Excel and Executor working properly!
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x000000E8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000076</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000005</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000005</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b0000</t>
+          <t>Binary: 0b0110</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Enhance authentication process with debug statements; update register encoding for consistency; improve memory read/write error handling; add simple example text file.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -542,7 +542,7 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x000000E8</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000076</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000010</t>
+          <t>Hex: 0x00000002</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000005</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000011</t>
+          <t>Hex: 0x00000003</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000005</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -838,7 +838,7 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000100</t>
+          <t>Hex: 0x00000004</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
@@ -930,7 +930,7 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Hex: 0x00000101</t>
+          <t>Hex: 0x00000005</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Hex: 0x00000110</t>
+          <t>Hex: 0x00000006</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>Hex: 0x00000111</t>
+          <t>Hex: 0x00000007</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>Hex: 0x00001000</t>
+          <t>Hex: 0x00000008</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b0110</t>
+          <t>Binary: 0b0000</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Final GUI integration, just testing remains
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -512,7 +512,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Int: 0d0</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000110</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000076</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000005</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000005</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b0000</t>
+          <t>Binary: 0b0110</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2542,7 +2542,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Binary: 0b11111111</t>
+          <t>Binary: 0b00000000</t>
         </is>
       </c>
       <c r="AB44" t="inlineStr">

</xml_diff>

<commit_message>
Refactor ALU arithmetic shift operation; improve signed handling and clarity. Update ControlUnit formatting. Adjust window position in config.json. Add example assembly code for testing.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -423,8 +423,8 @@
   </sheetPr>
   <dimension ref="A1:IP68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -552,7 +552,7 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000023</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000110</t>
+          <t>Hex: 0x00000098</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000076</t>
+          <t>Hex: 0x00000023</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000005</t>
+          <t>Hex: 0x00000023</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000023</t>
         </is>
       </c>
     </row>
@@ -818,7 +818,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000005</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b0110</t>
+          <t>Binary: 0b0000</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>String: 'NOP'</t>
+          <t>String: 'SWI'</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">

</xml_diff>

<commit_message>
Refactor Processor and PrinterUnit to include controller; update CPUView to pass controller during initialization. Adjust window position in config.json for better layout.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>Hex: 0x00000023</t>
+          <t>Hex: 0x0017AF25</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000098</t>
+          <t>Hex: 0x000000A0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000023</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000023</t>
+          <t>Hex: 0x0017AF25</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000023</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor and enhance security features across multiple modules
- Updated PrinterUnit.py to ensure consistent formatting and added newline at the end of the file.
- Modified Processor.py to improve register handling with additional newline for clarity.
- Enhanced SafeRegisters.py with detailed permission checks for read and write operations, ensuring security compliance.
- Refined VaultMemory.py to enforce access permissions and improve error handling during memory operations.
- Adjusted cpu_info_excel.py and table_control.py to standardize asset directory references from "Assets" to "assets".
- Updated various GUI components to reflect the new asset directory structure and improve file handling.
- Added a new assembly example (Seguridad.asm) to demonstrate logout and authentication processes.
- Updated configuration file paths in main.py to align with the new asset directory structure.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>Hex: 0x0017AF25</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000190</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000001</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000001</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000002</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000003</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -910,7 +910,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000004</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000005</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000006</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000007</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000008</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xF68C5A91</t>
         </is>
       </c>
       <c r="R11" s="1" t="n"/>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b0000</t>
+          <t>Binary: 0b0110</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2542,7 +2542,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Binary: 0b11111111</t>
+          <t>Binary: 0b00000000</t>
         </is>
       </c>
       <c r="AB44" t="inlineStr">

</xml_diff>

<commit_message>
Refactor memory write operations in LoginMemory and VaultMemory; add logging for write attempts and confirmations. Update CPUView to save vault and login memory states. Adjust window position in config.json for improved layout.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -522,7 +522,7 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000001</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000190</t>
+          <t>Hex: 0x00000178</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xDEADBEF0</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Hex: 0xF68C5A91</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="R11" s="1" t="n"/>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b0110</t>
+          <t>Binary: 0b1000</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Add new instruction encoding logic and update CPUView execution cycle handling; adjust window position in config.json for improved layout
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -522,7 +522,7 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>Hex: 0x00000001</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000178</t>
+          <t>Hex: 0x000001F0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xFFFFFFE1</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000100</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -828,7 +828,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xCA024636</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEF0</t>
+          <t>Hex: 0x14FD4D70</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xC6EF3720</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x4F1F3BA5</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xAB6FBBC0</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b1000</t>
+          <t>Binary: 0b1010</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Binary: 0b00</t>
+          <t>Binary: 0b11</t>
         </is>
       </c>
       <c r="Z23" s="1" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Binary: 0b00000000</t>
+          <t>Binary: 0b11111111</t>
         </is>
       </c>
       <c r="AB44" t="inlineStr">

</xml_diff>

<commit_message>
Refactor instruction encoding in encoder.py; reduce NOP instructions and correct register usage in ADD and SUB operations. Update window position in config.json for improved layout. Add new Decifrado_total.asm file for enhanced decryption logic.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x000001F0</t>
+          <t>Hex: 0x000003D0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Hex: 0xFFFFFFE1</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000100</t>
+          <t>Hex: 0x00000008</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -828,7 +828,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Hex: 0xCA024636</t>
+          <t>Hex: 0x616C6F48</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Hex: 0x14FD4D70</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Hex: 0xC6EF3720</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Hex: 0x4F1F3BA5</t>
+          <t>Hex: 0x9E3779B9</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Hex: 0xAB6FBBC0</t>
+          <t>Hex: 0xDEADBEEF</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b1010</t>
+          <t>Binary: 0b0110</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">

</xml_diff>

<commit_message>
Refactor DynamicMemory class for improved memory management; update CPUView to handle dynamic memory loading and saving. Adjust window position in config.json for better layout.
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x000003D0</t>
+          <t>Hex: 0x000003F0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000008</t>
+          <t>Hex: 0x00002CC0</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -828,7 +828,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Hex: 0x616C6F48</t>
+          <t>Hex: 0xE9836618</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x01C11FDB</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xC6EF3720</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Hex: 0x9E3779B9</t>
+          <t>Hex: 0x236F6748</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADBEEF</t>
+          <t>Hex: 0xE5F9DA1F</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">

</xml_diff>

<commit_message>
Refactor code structure for improved readability and maintainability. FINAL COMMIT
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0xAF250000</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x000003F0</t>
+          <t>Hex: 0x000003D0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000000</t>
+          <t>Hex: 0x00000017</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Hex: 0x00002CC0</t>
+          <t>Hex: 0x00000020</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -828,7 +828,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Hex: 0xE9836618</t>
+          <t>Hex: 0x696A2065</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Hex: 0x01C11FDB</t>
+          <t>Hex: 0x0000696A</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Hex: 0xC6EF3720</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Hex: 0x236F6748</t>
+          <t>Hex: 0x9E2E7496</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Hex: 0xE5F9DA1F</t>
+          <t>Hex: 0xDEADC23A</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">

</xml_diff>

<commit_message>
Arreglo gráfico que nisiquiera importa para la puntuación de nuestro simulador de CPU!
</commit_message>
<xml_diff>
--- a/ProyGrupal1/assets/table_data.xlsx
+++ b/ProyGrupal1/assets/table_data.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>Hex: 0xAF250000</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hex: 0x000003D0</t>
+          <t>Hex: 0x00000070</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000001</t>
+          <t>Hex: 0x00000096</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>Hex: 0x00000017</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000002</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Hex: 0x00000020</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Hex: 0x00000003</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -828,7 +828,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Hex: 0x696A2065</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -910,7 +910,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Hex: 0x00000004</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Hex: 0x0000696A</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Hex: 0x00000005</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Hex: 0x00000006</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Hex: 0x00000007</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Hex: 0x9E2E7496</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Hex: 0x00000008</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Hex: 0xDEADC23A</t>
+          <t>Hex: 0x00000000</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Binary: 0b0110</t>
+          <t>Binary: 0b0000</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Binary: 0b11</t>
+          <t>Binary: 0b00</t>
         </is>
       </c>
       <c r="Z23" s="1" t="n"/>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>String: 'NOP'</t>
+          <t>String: 'SWI'</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
@@ -2542,7 +2542,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Binary: 0b11111111</t>
+          <t>Binary: 0b00000000</t>
         </is>
       </c>
       <c r="AB44" t="inlineStr">

</xml_diff>